<commit_message>
modification de mon Compte Rendu
</commit_message>
<xml_diff>
--- a/Documentation/Fichiers personnelle/CR_Matthew_Flenet.xlsx
+++ b/Documentation/Fichiers personnelle/CR_Matthew_Flenet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84130D4D-24BF-4973-BB9D-F60992CB60E6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466FA1D6-38BB-4C2D-8234-074AC13ED1EA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="11">
   <si>
     <t>Compte Rendu - Matthew Flenet</t>
   </si>
@@ -101,31 +101,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF9FF4"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCB9AFC"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -227,37 +227,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -267,6 +249,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -561,7 +561,7 @@
   <dimension ref="B2:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,64 +573,64 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="7">
+      <c r="B4" s="14">
         <v>43756</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="3"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="7">
+      <c r="B5" s="14">
         <v>43756</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="3"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="10" t="s">
+      <c r="G5" s="16"/>
+      <c r="H5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="12"/>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="7">
+      <c r="B6" s="14">
         <v>43756</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
       <c r="E6" s="2"/>
       <c r="G6" s="3"/>
       <c r="H6" s="2" t="s">
@@ -638,186 +638,186 @@
       </c>
     </row>
     <row r="7" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
       <c r="E8" s="2"/>
-      <c r="I8" s="11"/>
+      <c r="I8" s="5"/>
     </row>
     <row r="9" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="8"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
       <c r="E10" s="2"/>
-      <c r="I10" s="11"/>
-      <c r="N10" s="11"/>
+      <c r="I10" s="5"/>
+      <c r="N10" s="5"/>
     </row>
     <row r="11" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="7"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="7"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="8"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="8"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="8"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="8"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="8"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="7"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="7"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="8"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="8"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="8"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="7"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="7"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
       <c r="E30" s="2"/>
     </row>
     <row r="31" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="8"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
       <c r="E31" s="2"/>
     </row>
     <row r="32" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="8"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
       <c r="E32" s="2"/>
     </row>
     <row r="33" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="8"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
       <c r="E33" s="2"/>
     </row>
     <row r="34" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="7"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
       <c r="E34" s="2"/>
     </row>
     <row r="35" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="7"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
       <c r="E35" s="2"/>
     </row>
     <row r="36" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="7"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
       <c r="E36" s="2"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>